<commit_message>
update stim list and exp with corrections
</commit_message>
<xml_diff>
--- a/exp/stim/trials/stim_list.xlsx
+++ b/exp/stim/trials/stim_list.xlsx
@@ -519,7 +519,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mariano hablaba del agua.</t>
+          <t>Mariano hablaba del tiempo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Manuela vendía el huevo.</t>
+          <t>Manuela vendía el carro</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Daniel iba a Bolivia</t>
+          <t>Daniel iba a Bolivia.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mariano hablaba del agua.</t>
+          <t>Mariano hablaba del tiempo.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -879,7 +879,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Manuela vendía el huevo.</t>
+          <t>Manuela vendía el carro.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -999,7 +999,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>¿Mariano hablaba del agua?</t>
+          <t>¿Mariano hablaba del tiempo?</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>¿Manuela vendía el huevo?</t>
+          <t>¿Manuela vendía el carro?</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>¿Por qué iba Daniel a Bolivia?</t>
+          <t>¿Por qué iba a Bolivia?</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>¿Cuándo leía David el libro?</t>
+          <t>¿Cuándo leía el libro?</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1209,7 +1209,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>¿Por qué ama Emilio la navidad?</t>
+          <t>¿Por qué ama la navidad?</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>¿Por qué hablaba Mariano del agua?</t>
+          <t>¿Por qué hablaba del agua?</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>¿Cuándo lleva Ana el abrigo?</t>
+          <t>¿Cuándo lleva el abrigo?</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -1299,7 +1299,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>¿Cuándo bebía María el vino?</t>
+          <t>¿Cuándo bebía el vino?</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1329,7 +1329,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>¿Por qué abre Olivia el regalo?</t>
+          <t>¿Por qué abre el regalo?</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>¿Cuándo vendía Manuela el huevo?</t>
+          <t>¿Cuándo vendía el carro?</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>La hermana lavaba el vidrio.</t>
+          <t>La hermana lavaba el plato.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Mi madre llama al niñero.</t>
+          <t>Mi madre llama al médico.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1539,7 +1539,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>El bebé bailaba muy bien.</t>
+          <t>El bebé comía muy bien.</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>La amiga vive en Orlando.</t>
+          <t>La amiga vive en Nueva York</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1599,7 +1599,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Mi novio venía al lago.</t>
+          <t>Mi novio viene del lago.</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1659,7 +1659,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>La hermana lavaba el vidrio.</t>
+          <t>La hermana lavaba el plato.</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1689,7 +1689,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Mi madre llama al niñero.</t>
+          <t>Mi madre llama al médico.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1774,12 +1774,12 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t xml:space="preserve">¿Cómo bailaba el bebé? </t>
+          <t xml:space="preserve">¿Cómo comía el bebé? </t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>El bebé bailaba muy bien.</t>
+          <t>El bebé comía muy bien.</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1809,7 +1809,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>La amiga vive en Orlando.</t>
+          <t>La amiga vive en Nueva York</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1834,12 +1834,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>¿A dónde venía tu novio?</t>
+          <t>¿De dónde viene tu novio?</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Mi novio venía al lago.</t>
+          <t>Mi novio viene del lago.</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>¿La hermana lavaba el vidrio?</t>
+          <t>¿La hermana lavaba el plato?</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>¿Mi madre llama al niñero?</t>
+          <t>¿Mi madre llama al médico?</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>¿El bebé bailaba muy bien?</t>
+          <t>¿El bebé comía muy bien?</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>¿La amiga vive en Orlando?</t>
+          <t>¿La amiga vive en Nueva York?</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2079,7 +2079,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>¿Mi novio venía al lago?</t>
+          <t>¿Mi novio viene del lago?</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>¿Cuándo mira el hombre la luna?</t>
+          <t>¿Cuándo mira la luna?</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2139,7 +2139,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>¿Cuándo lavaba la hermana el vidrio?</t>
+          <t>¿Cuándo lavaba el plato?</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>¿Cuándo llama mi madre al niñero?</t>
+          <t>¿Cuándo llama al médico?</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2199,7 +2199,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>¿Por qué oía el niño el río?</t>
+          <t>¿Por qué oía el río?</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>¿Por qué odia mi abuela a la reina?</t>
+          <t>¿Por qué odia a la reina?</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>¿Cuándo bailaba el bebé muy bien?</t>
+          <t>¿Cuándo comía muy bien?</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>¿Por qué vive la amiga en Orlando?</t>
+          <t>¿Por qué vive en Nueva York?</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>¿Por qué venía mi novio al lago?</t>
+          <t>¿Por qué viene del lago?</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">

</xml_diff>

<commit_message>
update stim list to include only 8 syllable utterances
</commit_message>
<xml_diff>
--- a/exp/stim/trials/stim_list.xlsx
+++ b/exp/stim/trials/stim_list.xlsx
@@ -429,7 +429,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Daniel iba a Bolivia</t>
+          <t>Daniel iba a Bolivia.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Emilio ama la navidad.</t>
+          <t>Emilio ama la marcha.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -519,7 +519,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mariano hablaba del tiempo</t>
+          <t>Mariano habla del tiempo.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -579,7 +579,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>María bebía el vino.</t>
+          <t>María bebe el vino.</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Olivia abre el regalo.</t>
+          <t>Marta abre el regalo.</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -639,7 +639,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Manuela vendía el carro</t>
+          <t>Manuela vende el carro.</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -729,7 +729,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Emilio ama la navidad.</t>
+          <t>Emilio ama la marcha.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -754,12 +754,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>¿De qué hablaba Mariano?</t>
+          <t>¿De qué habla Mariano?</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Mariano hablaba del tiempo.</t>
+          <t>Mariano habla del tiempo.</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -814,12 +814,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>¿Qué bebía María?</t>
+          <t>¿Qué bebe María?</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>María bebía el vino.</t>
+          <t>María bebe el vino.</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -844,12 +844,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>¿Qué abre Olivia?</t>
+          <t>¿Qué abre Marta?</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Olivia abre el regalo.</t>
+          <t>Marta abre el regalo.</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -874,12 +874,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>¿Qué vendía Manuela?</t>
+          <t>¿Qué vende Manuela?</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Manuela vendía el carro.</t>
+          <t>Manuela vende el carro.</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>¿Emilio ama la navidad?</t>
+          <t>¿Emilio ama la marcha?</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -999,7 +999,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>¿Mariano hablaba del tiempo?</t>
+          <t>¿Mariano habla del tiempo?</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1059,7 +1059,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>¿María bebía el vino?</t>
+          <t>¿María bebe el vino?</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1089,7 +1089,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>¿Olivia abre el regalo?</t>
+          <t>¿Marta abre el regalo?</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>¿Manuela vendía el carro?</t>
+          <t>¿Manuela vende el carro?</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1419,7 +1419,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>La hermana lavaba el plato.</t>
+          <t>La niña lava el plato.</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Mi madre llama al médico.</t>
+          <t>Mi madre come la fruta.</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1479,7 +1479,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>El niño oía el río.</t>
+          <t>El niño oye el río.</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1509,7 +1509,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>Mi abuela odia a la reina.</t>
+          <t>Mi tía odia la lluvia.</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>La amiga vive en Nueva York</t>
+          <t>La maestra vive en Paris.</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -1654,12 +1654,12 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>¿Qué lava la hermana?</t>
+          <t>¿Qué lava la niña?</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>La hermana lavaba el plato.</t>
+          <t>La niña lava el plato.</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1684,12 +1684,12 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>¿A quién llama tu madre?</t>
+          <t>¿Qué come tu madre?</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Mi madre llama al médico.</t>
+          <t>Mi madre come la fruta.</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -1714,12 +1714,12 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>¿Qué oía el niño?</t>
+          <t>¿Qué oye el niño?</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>El niño oía el río.</t>
+          <t>El niño oye el río.</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1744,12 +1744,12 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>¿A quién odia tu abuela?</t>
+          <t>¿Qué odia tu tía?</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Mi abuela odia a la reina.</t>
+          <t>Mi tía odia la lluvia.</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1804,12 +1804,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>¿En dónde vive la amiga?</t>
+          <t>¿Dónde vive la maestra?</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>La amiga vive en Nueva York</t>
+          <t>La maestra vive en Paris.</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -1899,7 +1899,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>¿La hermana lavaba el plato?</t>
+          <t>¿La niña lava el plato?</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -1929,7 +1929,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>¿Mi madre llama al médico?</t>
+          <t>¿Mi madre come la fruta?</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>¿El niño oía el río?</t>
+          <t>¿El niño oye el río?</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -1989,7 +1989,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>¿Mi abuela odia a la reina?</t>
+          <t>¿Mi tía odia la lluvia?</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2049,7 +2049,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>¿La amiga vive en Nueva York?</t>
+          <t>¿La maestra vive en Paris?</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>¿Cuándo mira la luna?</t>
+          <t>¿Cuándo miraba la luna?</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -2169,7 +2169,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>¿Cuándo llama al médico?</t>
+          <t>¿Cuándo comía la fruta?</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>¿Por qué odia a la reina?</t>
+          <t>¿Por qué odiaba la lluvia?</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -2259,7 +2259,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>¿Cuándo comía muy bien?</t>
+          <t>¿Por qué desayuna muy bien?</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>¿Por qué vive en Nueva York?</t>
+          <t>¿Por qué vivía en Paris?</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -2319,7 +2319,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>¿Por qué viene del lago?</t>
+          <t>¿Por qué venía del lago?</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">

</xml_diff>